<commit_message>
Offsets and other Exp2 data for P1 and P2
</commit_message>
<xml_diff>
--- a/Data/experimental design.xlsx
+++ b/Data/experimental design.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
   <si>
     <t>Participant</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>Done?</t>
+  </si>
+  <si>
+    <t>JG</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>DH</t>
   </si>
 </sst>
 </file>
@@ -470,7 +479,7 @@
   <dimension ref="B2:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,6 +532,9 @@
       <c r="N3">
         <v>7</v>
       </c>
+      <c r="P3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -564,6 +576,9 @@
       <c r="N4">
         <v>8</v>
       </c>
+      <c r="P4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -604,6 +619,9 @@
       </c>
       <c r="N5">
         <v>9</v>
+      </c>
+      <c r="P5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
started tagging for P4 - Exp 2
</commit_message>
<xml_diff>
--- a/Data/experimental design.xlsx
+++ b/Data/experimental design.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
   <si>
     <t>Participant</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>DH</t>
+  </si>
+  <si>
+    <t>SK</t>
   </si>
 </sst>
 </file>
@@ -479,7 +482,7 @@
   <dimension ref="B2:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,6 +666,9 @@
       </c>
       <c r="N6">
         <v>10</v>
+      </c>
+      <c r="P6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adding data to the exp1-consolidated
</commit_message>
<xml_diff>
--- a/Data/experimental design.xlsx
+++ b/Data/experimental design.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
   <si>
     <t>Participant</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Masa</t>
+  </si>
+  <si>
+    <t>Zahid</t>
   </si>
 </sst>
 </file>
@@ -491,7 +494,7 @@
   <dimension ref="B2:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="C10" sqref="C10:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,6 +854,9 @@
       </c>
       <c r="N10">
         <v>2</v>
+      </c>
+      <c r="P10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Exp2 for P8 P9 and P10
</commit_message>
<xml_diff>
--- a/Data/experimental design.xlsx
+++ b/Data/experimental design.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
   <si>
     <t>Participant</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>DG</t>
+  </si>
+  <si>
+    <t>AM</t>
   </si>
 </sst>
 </file>
@@ -500,7 +503,7 @@
   <dimension ref="B2:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,6 +995,9 @@
       </c>
       <c r="N13">
         <v>5</v>
+      </c>
+      <c r="P13" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
All data analysis, ready to write
</commit_message>
<xml_diff>
--- a/Data/experimental design.xlsx
+++ b/Data/experimental design.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
   <si>
     <t>Participant</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>AM</t>
+  </si>
+  <si>
+    <t>DR</t>
   </si>
 </sst>
 </file>
@@ -503,7 +506,7 @@
   <dimension ref="B2:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,6 +1042,9 @@
       </c>
       <c r="N14">
         <v>6</v>
+      </c>
+      <c r="P14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">

</xml_diff>